<commit_message>
Updates for regents testing
</commit_message>
<xml_diff>
--- a/app/data/RegentsCalendar.xlsx
+++ b/app/data/RegentsCalendar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekstampone/Library/Mobile Documents/com~apple~CloudDocs/Developer/data-specialist-flask/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880BC8BC-AD7C-A74A-8625-47706A0396E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C398C0A0-E582-CE4C-8A89-9D2BC4038FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="500" windowWidth="33560" windowHeight="28300" activeTab="2" xr2:uid="{98DCE2EE-096A-EF4C-9576-6BE138F05710}"/>
+    <workbookView xWindow="1700" yWindow="500" windowWidth="33560" windowHeight="28300" activeTab="3" xr2:uid="{98DCE2EE-096A-EF4C-9576-6BE138F05710}"/>
   </bookViews>
   <sheets>
     <sheet name="SectionProperties" sheetId="2" r:id="rId1"/>
@@ -13948,7 +13948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCA803E-0660-F641-BDDB-024EE43C3378}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
@@ -14150,8 +14150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF381A89-EC94-BD4E-AF94-947710DA3428}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14175,36 +14175,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>45679</v>
+        <v>45678</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>45679</v>
+        <v>45678</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -14212,101 +14212,101 @@
         <v>45678</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>26</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>45681</v>
+        <v>45679</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>135</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>45680</v>
+        <v>45679</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>45678</v>
+        <v>45679</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>45678</v>
+        <v>45679</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>45679</v>
+        <v>45680</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -14314,7 +14314,7 @@
         <v>45680</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>145</v>
@@ -14328,22 +14328,26 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>45679</v>
+        <v>45681</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>35</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E11">
+    <sortCondition ref="A2:A11"/>
+    <sortCondition ref="B2:B11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Family engagement and attendance jupiter summary
</commit_message>
<xml_diff>
--- a/app/data/RegentsCalendar.xlsx
+++ b/app/data/RegentsCalendar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekstampone/Library/Mobile Documents/com~apple~CloudDocs/Developer/data-specialist-flask/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C398C0A0-E582-CE4C-8A89-9D2BC4038FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FE5344-7614-8F4D-96DB-BF8815366FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1700" yWindow="500" windowWidth="33560" windowHeight="28300" activeTab="3" xr2:uid="{98DCE2EE-096A-EF4C-9576-6BE138F05710}"/>
   </bookViews>
@@ -16,13 +16,15 @@
     <sheet name="SectionProperties" sheetId="2" r:id="rId1"/>
     <sheet name="SummerSectionProperties" sheetId="4" r:id="rId2"/>
     <sheet name="2025-1" sheetId="6" r:id="rId3"/>
-    <sheet name="2024-1" sheetId="5" r:id="rId4"/>
-    <sheet name="2023-7" sheetId="3" r:id="rId5"/>
-    <sheet name="2023-2" sheetId="1" r:id="rId6"/>
+    <sheet name="2024-2" sheetId="7" r:id="rId4"/>
+    <sheet name="2024-1" sheetId="5" r:id="rId5"/>
+    <sheet name="2023-7" sheetId="3" r:id="rId6"/>
+    <sheet name="2023-2" sheetId="1" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'2023-2'!$A$1:$E$327</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'2023-7'!$A$1:$E$327</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'2023-2'!$A$1:$E$327</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'2023-7'!$A$1:$E$327</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2024-2'!$A$1:$E$327</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SummerSectionProperties!$A$1:$L$1004</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="168">
   <si>
     <t>Day</t>
   </si>
@@ -541,6 +543,15 @@
   </si>
   <si>
     <t>_</t>
+  </si>
+  <si>
+    <t>Bio</t>
+  </si>
+  <si>
+    <t>ESS</t>
+  </si>
+  <si>
+    <t>DistributedScoring</t>
   </si>
 </sst>
 </file>
@@ -633,7 +644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -645,6 +656,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13949,7 +13962,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14147,10 +14160,335 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F52638-A0BD-4648-8682-FCD1751FE67B}">
+  <dimension ref="A1:F265"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="11">
+        <v>45818</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
+        <v>45818</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="F3" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>45819</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>45825</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>45825</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>45826</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>45826</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>45828</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>45828</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>45832</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>45832</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>45833</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218" s="2"/>
+      <c r="B218" s="2"/>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A230" s="2"/>
+      <c r="B230" s="2"/>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A231" s="2"/>
+      <c r="B231" s="2"/>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A232" s="2"/>
+      <c r="B232" s="2"/>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A233" s="2"/>
+      <c r="B233" s="2"/>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A234" s="2"/>
+      <c r="B234" s="2"/>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A237" s="2"/>
+      <c r="B237" s="2"/>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A238" s="2"/>
+      <c r="B238" s="2"/>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A265" s="2"/>
+      <c r="B265" s="2"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F265">
+    <sortCondition ref="A2:A265"/>
+    <sortCondition ref="B2:B265"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF381A89-EC94-BD4E-AF94-947710DA3428}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -14352,7 +14690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B7BB07-9E9C-344A-8EF0-72CA0865EFBF}">
   <dimension ref="A1:E265"/>
   <sheetViews>
@@ -14568,7 +14906,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB66886-AAD9-A442-BF69-AADD50D3EDBE}">
   <dimension ref="A1:E265"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updates for Fall 2025
</commit_message>
<xml_diff>
--- a/app/data/RegentsCalendar.xlsx
+++ b/app/data/RegentsCalendar.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekstampone/Library/Mobile Documents/com~apple~CloudDocs/Developer/data-specialist-flask/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D46A80-55C8-7F43-A1A5-74A47DEC5A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B07981-5AB1-B145-A3DC-413968BB5D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="500" windowWidth="33560" windowHeight="28300" activeTab="1" xr2:uid="{98DCE2EE-096A-EF4C-9576-6BE138F05710}"/>
+    <workbookView xWindow="1700" yWindow="760" windowWidth="27880" windowHeight="18360" activeTab="2" xr2:uid="{98DCE2EE-096A-EF4C-9576-6BE138F05710}"/>
   </bookViews>
   <sheets>
     <sheet name="SectionProperties" sheetId="2" r:id="rId1"/>
     <sheet name="SummerSectionProperties" sheetId="4" r:id="rId2"/>
-    <sheet name="2024-7" sheetId="8" r:id="rId3"/>
-    <sheet name="2025-1" sheetId="6" r:id="rId4"/>
+    <sheet name="2025-1" sheetId="6" r:id="rId3"/>
+    <sheet name="2024-7" sheetId="8" r:id="rId4"/>
     <sheet name="2024-2" sheetId="7" r:id="rId5"/>
     <sheet name="2024-1" sheetId="5" r:id="rId6"/>
     <sheet name="2023-7" sheetId="3" r:id="rId7"/>
@@ -26,7 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'2023-2'!$A$1:$E$327</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'2023-7'!$A$1:$E$327</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'2024-2'!$A$1:$E$327</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2024-7'!$A$1:$E$326</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2024-7'!$A$1:$E$326</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SummerSectionProperties!$A$1:$K$1004</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="187">
   <si>
     <t>Day</t>
   </si>
@@ -602,6 +602,15 @@
   </si>
   <si>
     <t>_PM3</t>
+  </si>
+  <si>
+    <t>SXR2R</t>
+  </si>
+  <si>
+    <t>MXRJR</t>
+  </si>
+  <si>
+    <t>SXR3R</t>
   </si>
 </sst>
 </file>
@@ -1042,131 +1051,336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED29BD9C-93F7-3B47-BD2F-429330E86B98}">
-  <dimension ref="A1:E1004"/>
+  <dimension ref="A1:H1004"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>202</v>
+      </c>
+      <c r="D2">
+        <v>202</v>
+      </c>
+      <c r="E2">
+        <v>202</v>
+      </c>
+      <c r="F2">
+        <v>202</v>
+      </c>
+      <c r="G2">
+        <v>202</v>
+      </c>
+      <c r="H2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="3">
+        <v>940</v>
+      </c>
+      <c r="D3">
+        <v>801</v>
+      </c>
+      <c r="E3" s="3">
+        <v>940</v>
+      </c>
+      <c r="F3">
+        <v>801</v>
+      </c>
+      <c r="G3" s="3">
+        <v>646</v>
+      </c>
+      <c r="H3" s="3">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="3">
+        <v>925</v>
+      </c>
+      <c r="D4" s="3">
+        <v>802</v>
+      </c>
+      <c r="E4" s="3">
+        <v>925</v>
+      </c>
+      <c r="F4" s="3">
+        <v>802</v>
+      </c>
+      <c r="G4" s="3">
+        <v>645</v>
+      </c>
+      <c r="H4" s="3">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="3">
+        <v>923</v>
+      </c>
+      <c r="D5" s="3">
+        <v>822</v>
+      </c>
+      <c r="E5" s="3">
+        <v>923</v>
+      </c>
+      <c r="F5" s="3">
+        <v>822</v>
+      </c>
+      <c r="G5" s="3">
+        <v>640</v>
+      </c>
+      <c r="H5" s="3">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="3">
+        <v>921</v>
+      </c>
+      <c r="D6" s="3">
+        <v>824</v>
+      </c>
+      <c r="E6" s="3">
+        <v>921</v>
+      </c>
+      <c r="F6" s="3">
+        <v>824</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="3">
+        <v>902</v>
+      </c>
+      <c r="D7" s="3">
+        <v>826</v>
+      </c>
+      <c r="E7" s="3">
+        <v>902</v>
+      </c>
+      <c r="F7" s="3">
+        <v>826</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="3">
+        <v>906</v>
+      </c>
+      <c r="D8" s="3">
+        <v>840</v>
+      </c>
+      <c r="E8" s="3">
+        <v>906</v>
+      </c>
+      <c r="F8" s="3">
+        <v>840</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="3">
+        <v>845</v>
+      </c>
+      <c r="D9" s="3">
+        <v>845</v>
+      </c>
+      <c r="E9" s="3">
+        <v>845</v>
+      </c>
+      <c r="F9" s="3">
+        <v>845</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" s="3">
+        <v>840</v>
+      </c>
+      <c r="D10" s="3">
+        <v>902</v>
+      </c>
+      <c r="E10" s="3">
+        <v>840</v>
+      </c>
+      <c r="F10" s="3">
+        <v>902</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="3">
+        <v>826</v>
+      </c>
+      <c r="D11" s="3">
+        <v>906</v>
+      </c>
+      <c r="E11" s="3">
+        <v>826</v>
+      </c>
+      <c r="F11" s="3">
+        <v>906</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" s="3">
+        <v>806</v>
+      </c>
+      <c r="D12" s="3">
+        <v>806</v>
+      </c>
+      <c r="E12" s="3">
+        <v>806</v>
+      </c>
+      <c r="F12" s="3">
+        <v>806</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" s="3">
+        <v>202</v>
+      </c>
+      <c r="D13" s="3">
+        <v>202</v>
+      </c>
+      <c r="E13" s="3">
+        <v>202</v>
+      </c>
+      <c r="F13" s="3">
+        <v>202</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1174,137 +1388,397 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>329</v>
+      </c>
+      <c r="D16">
+        <v>329</v>
+      </c>
+      <c r="E16">
+        <v>329</v>
+      </c>
+      <c r="F16">
+        <v>329</v>
+      </c>
+      <c r="G16">
+        <v>329</v>
+      </c>
+      <c r="H16">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>329</v>
+      </c>
+      <c r="D17">
+        <v>329</v>
+      </c>
+      <c r="E17">
+        <v>329</v>
+      </c>
+      <c r="F17">
+        <v>329</v>
+      </c>
+      <c r="G17">
+        <v>329</v>
+      </c>
+      <c r="H17">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>329</v>
+      </c>
+      <c r="D18">
+        <v>329</v>
+      </c>
+      <c r="E18">
+        <v>329</v>
+      </c>
+      <c r="F18">
+        <v>329</v>
+      </c>
+      <c r="G18">
+        <v>329</v>
+      </c>
+      <c r="H18">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>329</v>
+      </c>
+      <c r="D19">
+        <v>329</v>
+      </c>
+      <c r="E19">
+        <v>329</v>
+      </c>
+      <c r="F19">
+        <v>329</v>
+      </c>
+      <c r="G19">
+        <v>329</v>
+      </c>
+      <c r="H19">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C20" s="6">
+        <v>725</v>
+      </c>
+      <c r="D20" s="6">
+        <v>726</v>
+      </c>
+      <c r="E20" s="6">
+        <v>522</v>
+      </c>
+      <c r="F20" s="6">
+        <v>529</v>
+      </c>
+      <c r="G20" s="6">
+        <v>219</v>
+      </c>
+      <c r="H20" s="6">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C21" s="7">
+        <v>701</v>
+      </c>
+      <c r="D21" s="7">
+        <v>702</v>
+      </c>
+      <c r="E21" s="7">
+        <v>523</v>
+      </c>
+      <c r="F21" s="7">
+        <v>540</v>
+      </c>
+      <c r="G21" s="7">
+        <v>219</v>
+      </c>
+      <c r="H21" s="7">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C22" s="7">
+        <v>701</v>
+      </c>
+      <c r="D22" s="7">
+        <v>702</v>
+      </c>
+      <c r="E22" s="7">
+        <v>523</v>
+      </c>
+      <c r="F22" s="7">
+        <v>540</v>
+      </c>
+      <c r="G22" s="7">
+        <v>219</v>
+      </c>
+      <c r="H22" s="7">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C23" s="7">
+        <v>701</v>
+      </c>
+      <c r="D23" s="7">
+        <v>702</v>
+      </c>
+      <c r="E23" s="7">
+        <v>523</v>
+      </c>
+      <c r="F23" s="7">
+        <v>540</v>
+      </c>
+      <c r="G23" s="7">
+        <v>219</v>
+      </c>
+      <c r="H23" s="7">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C24" s="8">
+        <v>722</v>
+      </c>
+      <c r="D24" s="8">
+        <v>724</v>
+      </c>
+      <c r="E24" s="8">
+        <v>524</v>
+      </c>
+      <c r="F24" s="8">
+        <v>542</v>
+      </c>
+      <c r="G24" s="8">
+        <v>225</v>
+      </c>
+      <c r="H24" s="8">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C25" s="8">
+        <v>722</v>
+      </c>
+      <c r="D25" s="8">
+        <v>724</v>
+      </c>
+      <c r="E25" s="8">
+        <v>524</v>
+      </c>
+      <c r="F25" s="8">
+        <v>542</v>
+      </c>
+      <c r="G25" s="8">
+        <v>225</v>
+      </c>
+      <c r="H25" s="8">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C26" s="9">
+        <v>740</v>
+      </c>
+      <c r="D26" s="9">
+        <v>742</v>
+      </c>
+      <c r="E26" s="9">
+        <v>525</v>
+      </c>
+      <c r="F26" s="9">
+        <v>544</v>
+      </c>
+      <c r="G26" s="9">
+        <v>227</v>
+      </c>
+      <c r="H26" s="9">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C27" s="9">
+        <v>740</v>
+      </c>
+      <c r="D27" s="9">
+        <v>742</v>
+      </c>
+      <c r="E27" s="9">
+        <v>525</v>
+      </c>
+      <c r="F27" s="9">
+        <v>544</v>
+      </c>
+      <c r="G27" s="9">
+        <v>227</v>
+      </c>
+      <c r="H27" s="9">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C28" s="10">
+        <v>743</v>
+      </c>
+      <c r="D28" s="10">
+        <v>744</v>
+      </c>
+      <c r="E28" s="10">
+        <v>527</v>
+      </c>
+      <c r="F28" s="10">
+        <v>545</v>
+      </c>
+      <c r="G28" s="10">
+        <v>229</v>
+      </c>
+      <c r="H28" s="10">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C29" s="10">
+        <v>743</v>
+      </c>
+      <c r="D29" s="10">
+        <v>744</v>
+      </c>
+      <c r="E29" s="10">
+        <v>527</v>
+      </c>
+      <c r="F29" s="10">
+        <v>545</v>
+      </c>
+      <c r="G29" s="10">
+        <v>229</v>
+      </c>
+      <c r="H29" s="10">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C31" s="7">
+        <v>321</v>
+      </c>
+      <c r="D31" s="7">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="3"/>
+      <c r="C32" s="7">
+        <v>321</v>
+      </c>
+      <c r="D32" s="7">
+        <v>321</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
@@ -1313,7 +1787,12 @@
       <c r="B33" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="3"/>
+      <c r="C33" s="7">
+        <v>321</v>
+      </c>
+      <c r="D33" s="7">
+        <v>321</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
@@ -1322,7 +1801,12 @@
       <c r="B34" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E34" s="3"/>
+      <c r="C34" s="8">
+        <v>319</v>
+      </c>
+      <c r="D34" s="8">
+        <v>319</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
@@ -1331,7 +1815,12 @@
       <c r="B35" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E35" s="3"/>
+      <c r="C35" s="8">
+        <v>319</v>
+      </c>
+      <c r="D35" s="8">
+        <v>319</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
@@ -1340,7 +1829,12 @@
       <c r="B36" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E36" s="3"/>
+      <c r="C36" s="9">
+        <v>323</v>
+      </c>
+      <c r="D36" s="9">
+        <v>323</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
@@ -1349,7 +1843,12 @@
       <c r="B37" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="3"/>
+      <c r="C37" s="9">
+        <v>323</v>
+      </c>
+      <c r="D37" s="9">
+        <v>323</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
@@ -1358,7 +1857,12 @@
       <c r="B38" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E38" s="3"/>
+      <c r="C38" s="10">
+        <v>327</v>
+      </c>
+      <c r="D38" s="10">
+        <v>327</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
@@ -1367,7 +1871,12 @@
       <c r="B39" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="3"/>
+      <c r="C39" s="10">
+        <v>327</v>
+      </c>
+      <c r="D39" s="10">
+        <v>327</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
@@ -1376,7 +1885,6 @@
       <c r="B40" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="3"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
@@ -1385,7 +1893,12 @@
       <c r="B41" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E41" s="3"/>
+      <c r="C41" s="7">
+        <v>701</v>
+      </c>
+      <c r="E41" s="7">
+        <v>701</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
@@ -1394,7 +1907,12 @@
       <c r="B42" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E42" s="3"/>
+      <c r="C42" s="7">
+        <v>701</v>
+      </c>
+      <c r="E42" s="7">
+        <v>701</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
@@ -1403,7 +1921,12 @@
       <c r="B43" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E43" s="3"/>
+      <c r="C43" s="7">
+        <v>701</v>
+      </c>
+      <c r="E43" s="7">
+        <v>701</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
@@ -1412,7 +1935,12 @@
       <c r="B44" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E44" s="3"/>
+      <c r="C44" s="8">
+        <v>722</v>
+      </c>
+      <c r="E44" s="8">
+        <v>722</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
@@ -1421,7 +1949,12 @@
       <c r="B45" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E45" s="3"/>
+      <c r="C45" s="8">
+        <v>722</v>
+      </c>
+      <c r="E45" s="8">
+        <v>722</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
@@ -1430,7 +1963,12 @@
       <c r="B46" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E46" s="3"/>
+      <c r="C46" s="9">
+        <v>740</v>
+      </c>
+      <c r="E46" s="9">
+        <v>740</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
@@ -1439,7 +1977,12 @@
       <c r="B47" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E47" s="3"/>
+      <c r="C47" s="9">
+        <v>740</v>
+      </c>
+      <c r="E47" s="9">
+        <v>740</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
@@ -1448,99 +1991,162 @@
       <c r="B48" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E48" s="3"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C48" s="10">
+        <v>743</v>
+      </c>
+      <c r="E48" s="10">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E49" s="3"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C49" s="10">
+        <v>743</v>
+      </c>
+      <c r="E49" s="10">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E50" s="3"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C51" s="7">
+        <v>701</v>
+      </c>
+      <c r="F51" s="7">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C52" s="7">
+        <v>701</v>
+      </c>
+      <c r="F52" s="7">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C53" s="7">
+        <v>701</v>
+      </c>
+      <c r="F53" s="7">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C54" s="8">
+        <v>722</v>
+      </c>
+      <c r="F54" s="8">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C55" s="8">
+        <v>722</v>
+      </c>
+      <c r="F55" s="8">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C56" s="9">
+        <v>740</v>
+      </c>
+      <c r="F56" s="9">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C57" s="9">
+        <v>740</v>
+      </c>
+      <c r="F57" s="9">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C58" s="10">
+        <v>743</v>
+      </c>
+      <c r="F58" s="10">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C59" s="10">
+        <v>743</v>
+      </c>
+      <c r="F59" s="10">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -1548,75 +2154,129 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>60</v>
       </c>
       <c r="B61" s="3"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D61" s="7">
+        <v>702</v>
+      </c>
+      <c r="E61" s="7">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>61</v>
       </c>
       <c r="B62" s="3"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D62" s="7">
+        <v>702</v>
+      </c>
+      <c r="E62" s="7">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D63" s="7">
+        <v>702</v>
+      </c>
+      <c r="E63" s="7">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D64" s="8">
+        <v>724</v>
+      </c>
+      <c r="E64" s="8">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D65" s="8">
+        <v>724</v>
+      </c>
+      <c r="E65" s="8">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D66" s="9">
+        <v>742</v>
+      </c>
+      <c r="E66" s="9">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D67" s="9">
+        <v>742</v>
+      </c>
+      <c r="E67" s="9">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D68" s="10">
+        <v>744</v>
+      </c>
+      <c r="E68" s="10">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D69" s="10">
+        <v>744</v>
+      </c>
+      <c r="E69" s="10">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -1624,125 +2284,287 @@
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>70</v>
       </c>
       <c r="B71" s="3"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D71" s="7">
+        <v>702</v>
+      </c>
+      <c r="F71" s="7">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>71</v>
       </c>
       <c r="B72" s="3"/>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D72" s="7">
+        <v>702</v>
+      </c>
+      <c r="F72" s="7">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>72</v>
       </c>
       <c r="B73" s="3"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D73" s="7">
+        <v>702</v>
+      </c>
+      <c r="F73" s="7">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>73</v>
       </c>
       <c r="B74" s="3"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D74" s="8">
+        <v>724</v>
+      </c>
+      <c r="F74" s="8">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>74</v>
       </c>
       <c r="B75" s="3"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D75" s="8">
+        <v>724</v>
+      </c>
+      <c r="F75" s="8">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>75</v>
       </c>
       <c r="B76" s="3"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D76" s="9">
+        <v>742</v>
+      </c>
+      <c r="F76" s="9">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>76</v>
       </c>
       <c r="B77" s="3"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D77" s="9">
+        <v>742</v>
+      </c>
+      <c r="F77" s="9">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>77</v>
       </c>
       <c r="B78" s="3"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D78" s="10">
+        <v>744</v>
+      </c>
+      <c r="F78" s="10">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>78</v>
       </c>
       <c r="B79" s="3"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D79" s="10">
+        <v>744</v>
+      </c>
+      <c r="F79" s="10">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>79</v>
       </c>
       <c r="B80" s="3"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>80</v>
       </c>
       <c r="B81" s="3"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D81">
+        <v>202</v>
+      </c>
+      <c r="E81">
+        <v>202</v>
+      </c>
+      <c r="F81">
+        <v>202</v>
+      </c>
+      <c r="G81">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>81</v>
       </c>
       <c r="B82" s="3"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D82">
+        <v>202</v>
+      </c>
+      <c r="E82">
+        <v>202</v>
+      </c>
+      <c r="F82">
+        <v>202</v>
+      </c>
+      <c r="G82">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>82</v>
       </c>
       <c r="B83" s="3"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D83">
+        <v>202</v>
+      </c>
+      <c r="E83">
+        <v>202</v>
+      </c>
+      <c r="F83">
+        <v>202</v>
+      </c>
+      <c r="G83">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>83</v>
       </c>
       <c r="B84" s="3"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D84">
+        <v>202</v>
+      </c>
+      <c r="E84">
+        <v>202</v>
+      </c>
+      <c r="F84">
+        <v>202</v>
+      </c>
+      <c r="G84">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>84</v>
       </c>
       <c r="B85" s="3"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D85">
+        <v>202</v>
+      </c>
+      <c r="E85">
+        <v>202</v>
+      </c>
+      <c r="F85">
+        <v>202</v>
+      </c>
+      <c r="G85">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>85</v>
       </c>
       <c r="B86" s="3"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D86">
+        <v>202</v>
+      </c>
+      <c r="E86">
+        <v>202</v>
+      </c>
+      <c r="F86">
+        <v>202</v>
+      </c>
+      <c r="G86">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>86</v>
       </c>
       <c r="B87" s="3"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D87">
+        <v>202</v>
+      </c>
+      <c r="E87">
+        <v>202</v>
+      </c>
+      <c r="F87">
+        <v>202</v>
+      </c>
+      <c r="G87">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>87</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D88">
+        <v>202</v>
+      </c>
+      <c r="E88">
+        <v>202</v>
+      </c>
+      <c r="F88">
+        <v>202</v>
+      </c>
+      <c r="G88">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>88</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D89">
+        <v>202</v>
+      </c>
+      <c r="E89">
+        <v>202</v>
+      </c>
+      <c r="F89">
+        <v>202</v>
+      </c>
+      <c r="G89">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -1750,91 +2572,118 @@
         <v>129</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H91" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H92" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H93" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H94" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H95" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H96" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H97" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H98" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H99" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
     </row>
@@ -5407,6 +6256,18 @@
       <c r="B1004" s="3"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C3:F12">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -5416,8 +6277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6309B1-B2F2-C24D-9683-349831E0A64F}">
   <dimension ref="A1:V1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="R100" sqref="R100"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13493,12 +14354,270 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCA803E-0660-F641-BDDB-024EE43C3378}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>46042</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>46042</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>46042</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>46042</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>46043</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>46043</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>46043</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>46043</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>46044</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>46044</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>46045</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>46045</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E264">
+    <sortCondition ref="A2:A264"/>
+    <sortCondition ref="B2:B264"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517AF821-DE73-E44B-B05F-E5374FFCFDC2}">
   <dimension ref="A1:F264"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13769,208 +14888,6 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCA803E-0660-F641-BDDB-024EE43C3378}">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>45679</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>45679</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>45678</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>45681</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>45680</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>45678</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>45678</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>45679</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>45680</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>45679</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updates to Jupiter, teacher analysis, etc
</commit_message>
<xml_diff>
--- a/app/data/RegentsCalendar.xlsx
+++ b/app/data/RegentsCalendar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekstampone/Library/Mobile Documents/com~apple~CloudDocs/Developer/data-specialist-flask/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B07981-5AB1-B145-A3DC-413968BB5D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A578EA1-53E3-6C4E-A067-E83ACCA3B152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1700" yWindow="760" windowWidth="27880" windowHeight="18360" activeTab="2" xr2:uid="{98DCE2EE-096A-EF4C-9576-6BE138F05710}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="190">
   <si>
     <t>Day</t>
   </si>
@@ -611,6 +611,15 @@
   </si>
   <si>
     <t>SXR3R</t>
+  </si>
+  <si>
+    <t>SBS43</t>
+  </si>
+  <si>
+    <t>MRS41</t>
+  </si>
+  <si>
+    <t>SJS43</t>
   </si>
 </sst>
 </file>
@@ -14358,7 +14367,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14437,6 +14446,9 @@
       <c r="D4" s="3" t="s">
         <v>160</v>
       </c>
+      <c r="E4" t="s">
+        <v>187</v>
+      </c>
       <c r="F4" s="3">
         <v>2</v>
       </c>
@@ -14508,7 +14520,9 @@
       <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="F8" s="3">
         <v>1</v>
       </c>
@@ -14597,7 +14611,9 @@
       <c r="D13" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>189</v>
+      </c>
       <c r="F13" s="3">
         <v>1</v>
       </c>

</xml_diff>